<commit_message>
Config changes and addition of sql queries in excel file
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="372" windowWidth="22980" windowHeight="9228" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="372" windowWidth="22980" windowHeight="9228" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="83">
   <si>
     <t>City</t>
   </si>
@@ -357,21 +357,80 @@
 where p.EMAIL_ADR_TXT='{$email}' and pv.PAY_PROC_CD_DESC='User Type Code'</t>
   </si>
   <si>
-    <t>select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
-on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
-where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in( '{$id}' )</t>
-  </si>
-  <si>
     <t>select * from  OLE.PORTAL_USER p join OLE.portal_user_tin pt 
 on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
 where p.USERNAME='{$user}'and pt.PROV_TIN_NBR='{$tinNo}' and CNTC_ROLE_CD='A'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AUBILL5903 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select * from  OLE.PORTAL_USER p where p.EMAIL_ADR_TXT='{$email}'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutomationBilling                                                                                   </t>
+  </si>
+  <si>
+    <t>AUPAYE5365</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AutomationPayer                                                                                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+ select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_PAYER_TIN pt 
+  on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where p.EMAIL_ADR_TXT='{$email}' and pt.PAYR_TIN_NBR='{$tinNo}'</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> select * from  OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
+  on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
+  on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
+where p.EMAIL_ADR_TXT='{$email}'and bs.IDENTIFIER_NBR='{$tinNo}'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  select * from OLE.ENROLLED_PROVIDER p where p.ENRL_STS_CD='A' 
+  order by p.CREAT_DTTM desc FETCH FIRST 1 ROW ONLY </t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  select * from OLE.BILLING_SERVICE bs where bs.ENRL_STS_CD='A' 
+  order by bs.ENRL_DTTM desc FETCH FIRST 1 ROW ONLY </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  select * from OLE.Payer p where p.PAYR_ACTV_IND='Y' 
+  order by p.CREAT_DTTM desc FETCH FIRST 1 ROW ONLY </t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
+on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
+where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in( '{$id}' ) and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365')
+</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  
+select * from OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
+on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
+ on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
+where  bs.IDENTIFIER_NBR='{$tin}'  and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +442,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -405,10 +479,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -427,8 +502,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1151,10 +1229,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,12 +1334,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1269,16 +1347,71 @@
         <v>35</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B17" s="6" t="s">
+      <c r="B13" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="5"/>
+      <c r="B20" s="7"/>
+    </row>
+    <row r="21" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="6" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1292,7 +1425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1423,15 +1556,54 @@
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>31</v>
       </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" t="s">
+        <v>71</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F8" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Config changes and test base class changes to handle in case test suite or env is null from jenkins
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFile.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="85">
   <si>
     <t>City</t>
   </si>
@@ -410,20 +410,29 @@
     <t>17</t>
   </si>
   <si>
+    <t>18</t>
+  </si>
+  <si>
     <t xml:space="preserve">select * from OLE.PORTAL_USER p join OLE.portal_user_tin pt 
 on p.PORTAL_USER_ID=pt.PORTAL_USER_ID
-where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in( '{$id}' ) and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365')
+where pt.PROV_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in( '{$id}' ) and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc
 </t>
   </si>
   <si>
-    <t>18</t>
+    <t>select * from OLE.PORTAL_USER p join
+OLE.PORTAL_USER_PAYER_TIN py 
+on p.PORTAL_USER_ID=py.PORTAL_USER_ID 
+where  py.PAYR_TIN_NBR='{$tin}' and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>19</t>
   </si>
   <si>
     <t xml:space="preserve">  
 select * from OLE.PORTAL_USER p join OLE.PORTAL_USER_BS_TIN bt 
 on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
  on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
-where  bs.IDENTIFIER_NBR='{$tin}'  and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365')</t>
+where  bs.IDENTIFIER_NBR='{$tin}'  and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
   </si>
 </sst>
 </file>
@@ -1231,7 +1240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1334,12 +1343,12 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -1398,17 +1407,21 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="7"/>
     </row>
     <row r="21" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">

</xml_diff>

<commit_message>
vo test case was missed , added that
</commit_message>
<xml_diff>
--- a/Online-Portals/UPA/DataFile.xlsx
+++ b/Online-Portals/UPA/DataFile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="372" windowWidth="22980" windowHeight="9228" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="372" windowWidth="22980" windowHeight="9228"/>
   </bookViews>
   <sheets>
     <sheet name="FinancialInfo" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="86">
   <si>
     <t>City</t>
   </si>
@@ -433,6 +433,9 @@
 on p.PORTAL_USER_ID=bt.PORTAL_USER_ID join OLE.BILLING_SERVICE bs
  on bt.BILLING_SERVICE_ID=bs.BILLING_SERVICE_ID
 where  bs.IDENTIFIER_NBR='{$tin}'  and p.STS_CD='A' and p.USERNAME not in ('USPROV7729','AUAUTO1563','AUAUTO5896','AUBILL5903','AUPAYE5365') order by p.LST_CHG_BY_DTTM desc Fetch FIRST ROW ONLY</t>
+  </si>
+  <si>
+    <t>VO</t>
   </si>
 </sst>
 </file>
@@ -817,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -967,7 +970,10 @@
         <v>26</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>29</v>
+        <v>85</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1240,7 +1246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>

</xml_diff>